<commit_message>
added ROC AUC to gradient boosted decision trees
</commit_message>
<xml_diff>
--- a/Zahin Ahmed/GB_parameter_tuning.xlsx
+++ b/Zahin Ahmed/GB_parameter_tuning.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>n_estimators</t>
   </si>
@@ -27,9 +28,6 @@
     <t>max_features</t>
   </si>
   <si>
-    <t>Input_Feature</t>
-  </si>
-  <si>
     <t>Antibiotic</t>
   </si>
   <si>
@@ -60,34 +58,22 @@
     <t>TP</t>
   </si>
   <si>
-    <t>S.PRC</t>
-  </si>
-  <si>
-    <t>S.RCL</t>
-  </si>
-  <si>
-    <t>R.PRC</t>
-  </si>
-  <si>
-    <t>R.RCL</t>
-  </si>
-  <si>
-    <t>S.FSc</t>
-  </si>
-  <si>
-    <t>R.FSc</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
     <t>AMX</t>
   </si>
   <si>
-    <t>GYS</t>
-  </si>
-  <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>Sensitivity (TPR)</t>
+  </si>
+  <si>
+    <t>Specificty(TNR)</t>
+  </si>
+  <si>
+    <t>1-Specificity(FPR)</t>
   </si>
 </sst>
 </file>
@@ -405,28 +391,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,91 +452,120 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>600</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
       </c>
       <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>0.8</v>
+      </c>
+      <c r="I2">
+        <v>72</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>15</v>
+      </c>
+      <c r="L2">
+        <v>120</v>
+      </c>
+      <c r="M2">
+        <f>L2/(L2+K2)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="N2">
+        <f>I2/(I2+J2)</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="O2">
+        <f>1-N2</f>
+        <v>0.1428571428571429</v>
+      </c>
+      <c r="P2">
+        <f>((I2+L2)/SUM(I2:L2))</f>
+        <v>0.87671232876712324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>300</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
         <v>0.1</v>
       </c>
-      <c r="F2">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="I2">
+      <c r="H3">
         <v>0.8</v>
       </c>
-      <c r="J2">
-        <v>72</v>
-      </c>
-      <c r="K2">
-        <v>12</v>
-      </c>
-      <c r="L2">
-        <v>15</v>
-      </c>
-      <c r="M2">
-        <v>120</v>
-      </c>
-      <c r="N2">
-        <v>0.83</v>
-      </c>
-      <c r="O2">
-        <v>0.86</v>
-      </c>
-      <c r="P2">
-        <v>0.91</v>
-      </c>
-      <c r="Q2">
-        <v>0.89</v>
-      </c>
-      <c r="R2">
-        <v>0.84</v>
-      </c>
-      <c r="S2">
-        <v>0.9</v>
-      </c>
-      <c r="T2">
-        <f>((J2+M2)/SUM(J2:M2))</f>
-        <v>0.87671232876712324</v>
+      <c r="I3">
+        <v>75</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>119</v>
+      </c>
+      <c r="M3">
+        <f>L3/(L3+K3)</f>
+        <v>0.88148148148148153</v>
+      </c>
+      <c r="N3">
+        <f>I3/(I3+J3)</f>
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="O3">
+        <f>1-N3</f>
+        <v>0.1071428571428571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>